<commit_message>
Updated Gantt Chart + Tidied for Submission
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathanael\Desktop\Uni Trim 2 2023\2810 Software Technologies\Repository\2810ICT-7810ICT-2023-Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13209926-3B7A-4D50-ADA8-B2617CC7DF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF140EC-2EBA-44CE-A87E-E07ECE5E4CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="66">
   <si>
     <t>ID</t>
   </si>
@@ -221,10 +221,16 @@
     <t>-</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Duration (days)</t>
+  </si>
+  <si>
+    <t>6.2</t>
+  </si>
+  <si>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>Week 8</t>
   </si>
 </sst>
 </file>
@@ -575,21 +581,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -625,16 +616,25 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -642,7 +642,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -678,9 +678,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -690,7 +687,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -725,114 +722,6 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="14" borderId="18" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -842,18 +731,185 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1182,10 +1238,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AQ45"/>
+  <dimension ref="A1:BB46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AY18" sqref="AY18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18:AY18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -1193,80 +1249,96 @@
     <col min="1" max="1" width="10" style="3" customWidth="1"/>
     <col min="2" max="2" width="50" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="67" width="5.7109375" customWidth="1"/>
+    <col min="4" max="47" width="5.7109375" customWidth="1"/>
+    <col min="48" max="48" width="5.7109375" style="3" customWidth="1"/>
+    <col min="49" max="67" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="19" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="84" t="s">
+    <row r="1" spans="1:54" s="16" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="83" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" s="78" t="s">
+      <c r="C1" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="78" t="s">
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="78" t="s">
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="80"/>
-      <c r="S1" s="78" t="s">
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="T1" s="79"/>
-      <c r="U1" s="79"/>
-      <c r="V1" s="79"/>
-      <c r="W1" s="80"/>
-      <c r="X1" s="78" t="s">
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="39"/>
+      <c r="X1" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="Y1" s="79"/>
-      <c r="Z1" s="79"/>
-      <c r="AA1" s="79"/>
-      <c r="AB1" s="80"/>
-      <c r="AC1" s="78" t="s">
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="39"/>
+      <c r="AC1" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="AD1" s="79"/>
-      <c r="AE1" s="79"/>
-      <c r="AF1" s="79"/>
-      <c r="AG1" s="80"/>
-      <c r="AH1" s="78" t="s">
+      <c r="AD1" s="38"/>
+      <c r="AE1" s="38"/>
+      <c r="AF1" s="38"/>
+      <c r="AG1" s="39"/>
+      <c r="AH1" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="AI1" s="79"/>
-      <c r="AJ1" s="79"/>
-      <c r="AK1" s="79"/>
-      <c r="AL1" s="80"/>
-      <c r="AM1" s="78" t="s">
+      <c r="AI1" s="38"/>
+      <c r="AJ1" s="38"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="39"/>
+      <c r="AM1" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="AN1" s="79"/>
-      <c r="AO1" s="79"/>
-      <c r="AP1" s="79"/>
-      <c r="AQ1" s="80"/>
-    </row>
-    <row r="2" spans="1:43" s="19" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="84"/>
-      <c r="B2" s="81"/>
-      <c r="C2" s="83"/>
+      <c r="AN1" s="38"/>
+      <c r="AO1" s="38"/>
+      <c r="AP1" s="38"/>
+      <c r="AQ1" s="39"/>
+      <c r="AR1" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="AS1" s="38"/>
+      <c r="AT1" s="38"/>
+      <c r="AU1" s="38"/>
+      <c r="AV1" s="39"/>
+      <c r="AW1" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="AX1" s="38"/>
+      <c r="AY1" s="38"/>
+      <c r="AZ1" s="38"/>
+      <c r="BA1" s="39"/>
+    </row>
+    <row r="2" spans="1:54" s="16" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="41"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="40"/>
       <c r="D2" s="2" t="s">
         <v>51</v>
       </c>
@@ -1387,67 +1459,109 @@
       <c r="AQ2" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:43" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="31" t="s">
+      <c r="AR2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AT2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AV2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AX2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AY2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AZ2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BA2" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="20" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="82"/>
-      <c r="N3" s="82"/>
-      <c r="O3" s="82"/>
-      <c r="P3" s="82"/>
-      <c r="Q3" s="82"/>
-      <c r="R3" s="82"/>
-      <c r="S3" s="82"/>
-      <c r="T3" s="82"/>
-      <c r="U3" s="82"/>
-      <c r="V3" s="82"/>
-      <c r="W3" s="82"/>
-      <c r="X3" s="82"/>
-      <c r="Y3" s="82"/>
-      <c r="Z3" s="82"/>
-      <c r="AA3" s="82"/>
-      <c r="AB3" s="82"/>
-      <c r="AC3" s="82"/>
-      <c r="AD3" s="82"/>
-      <c r="AE3" s="82"/>
-      <c r="AF3" s="82"/>
-      <c r="AG3" s="82"/>
-      <c r="AH3" s="82"/>
-      <c r="AI3" s="82"/>
-      <c r="AJ3" s="82"/>
-      <c r="AK3" s="82"/>
-      <c r="AL3" s="82"/>
-      <c r="AM3" s="82"/>
-      <c r="AN3" s="82"/>
-      <c r="AO3" s="82"/>
-      <c r="AQ3" s="18"/>
-    </row>
-    <row r="4" spans="1:43" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="32">
+      <c r="D3" s="78"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79"/>
+      <c r="O3" s="79"/>
+      <c r="P3" s="79"/>
+      <c r="Q3" s="79"/>
+      <c r="R3" s="79"/>
+      <c r="S3" s="79"/>
+      <c r="T3" s="79"/>
+      <c r="U3" s="79"/>
+      <c r="V3" s="79"/>
+      <c r="W3" s="79"/>
+      <c r="X3" s="79"/>
+      <c r="Y3" s="79"/>
+      <c r="Z3" s="79"/>
+      <c r="AA3" s="79"/>
+      <c r="AB3" s="79"/>
+      <c r="AC3" s="79"/>
+      <c r="AD3" s="79"/>
+      <c r="AE3" s="79"/>
+      <c r="AF3" s="79"/>
+      <c r="AG3" s="79"/>
+      <c r="AH3" s="79"/>
+      <c r="AI3" s="79"/>
+      <c r="AJ3" s="79"/>
+      <c r="AK3" s="79"/>
+      <c r="AL3" s="79"/>
+      <c r="AM3" s="79"/>
+      <c r="AN3" s="79"/>
+      <c r="AO3" s="79"/>
+      <c r="AP3" s="79"/>
+      <c r="AQ3" s="79"/>
+      <c r="AR3" s="79"/>
+      <c r="AS3" s="79"/>
+      <c r="AT3" s="79"/>
+      <c r="AU3" s="79"/>
+      <c r="AV3" s="79"/>
+      <c r="AW3" s="79"/>
+      <c r="AX3" s="79"/>
+      <c r="AY3" s="80"/>
+      <c r="AZ3" s="18"/>
+      <c r="BA3" s="18"/>
+      <c r="BB3" s="97"/>
+    </row>
+    <row r="4" spans="1:54" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="21" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5">
         <v>2</v>
       </c>
-      <c r="F4" s="74"/>
-      <c r="G4" s="75"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="47"/>
       <c r="H4" s="3"/>
       <c r="M4" s="3"/>
       <c r="R4" s="3"/>
@@ -1456,63 +1570,74 @@
       <c r="AG4" s="3"/>
       <c r="AL4" s="3"/>
       <c r="AQ4" s="3"/>
-    </row>
-    <row r="5" spans="1:43" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="33">
+      <c r="BA4" s="3"/>
+    </row>
+    <row r="5" spans="1:54" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="30">
         <v>1.2</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="17">
         <v>1</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
       <c r="F5" s="12"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="22"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="21"/>
-      <c r="W5" s="22"/>
-      <c r="X5" s="21"/>
-      <c r="Y5" s="21"/>
-      <c r="Z5" s="21"/>
-      <c r="AA5" s="21"/>
-      <c r="AB5" s="22"/>
-      <c r="AC5" s="21"/>
-      <c r="AD5" s="21"/>
-      <c r="AE5" s="21"/>
-      <c r="AF5" s="21"/>
-      <c r="AG5" s="22"/>
-      <c r="AH5" s="21"/>
-      <c r="AI5" s="21"/>
-      <c r="AJ5" s="21"/>
-      <c r="AK5" s="21"/>
-      <c r="AL5" s="22"/>
-      <c r="AM5" s="21"/>
-      <c r="AN5" s="21"/>
-      <c r="AO5" s="21"/>
-      <c r="AP5" s="21"/>
-      <c r="AQ5" s="22"/>
-    </row>
-    <row r="6" spans="1:43" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="32">
+      <c r="G5" s="18"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="18"/>
+      <c r="U5" s="18"/>
+      <c r="V5" s="18"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="18"/>
+      <c r="Y5" s="18"/>
+      <c r="Z5" s="18"/>
+      <c r="AA5" s="18"/>
+      <c r="AB5" s="19"/>
+      <c r="AC5" s="18"/>
+      <c r="AD5" s="18"/>
+      <c r="AE5" s="18"/>
+      <c r="AF5" s="18"/>
+      <c r="AG5" s="19"/>
+      <c r="AH5" s="18"/>
+      <c r="AI5" s="18"/>
+      <c r="AJ5" s="18"/>
+      <c r="AK5" s="18"/>
+      <c r="AL5" s="19"/>
+      <c r="AM5" s="18"/>
+      <c r="AN5" s="18"/>
+      <c r="AO5" s="18"/>
+      <c r="AP5" s="18"/>
+      <c r="AQ5" s="19"/>
+      <c r="AR5" s="18"/>
+      <c r="AS5" s="18"/>
+      <c r="AT5" s="18"/>
+      <c r="AU5" s="18"/>
+      <c r="AV5" s="19"/>
+      <c r="AW5" s="18"/>
+      <c r="AX5" s="18"/>
+      <c r="AY5" s="18"/>
+      <c r="AZ5" s="18"/>
+      <c r="BA5" s="19"/>
+    </row>
+    <row r="6" spans="1:54" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="29">
         <v>1.3</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="5">
@@ -1527,33 +1652,36 @@
       <c r="AG6" s="3"/>
       <c r="AL6" s="3"/>
       <c r="AQ6" s="3"/>
-    </row>
-    <row r="7" spans="1:43" s="21" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="33">
+      <c r="BA6" s="3"/>
+    </row>
+    <row r="7" spans="1:54" s="18" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="30">
         <v>1.4</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="17">
         <v>2</v>
       </c>
-      <c r="D7" s="67"/>
-      <c r="E7" s="68"/>
-      <c r="H7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="R7" s="22"/>
-      <c r="W7" s="22"/>
-      <c r="AB7" s="22"/>
-      <c r="AG7" s="22"/>
-      <c r="AL7" s="22"/>
-      <c r="AQ7" s="22"/>
-    </row>
-    <row r="8" spans="1:43" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="32">
+      <c r="D7" s="42"/>
+      <c r="E7" s="44"/>
+      <c r="H7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="W7" s="19"/>
+      <c r="AB7" s="19"/>
+      <c r="AG7" s="19"/>
+      <c r="AL7" s="19"/>
+      <c r="AQ7" s="19"/>
+      <c r="AV7" s="19"/>
+      <c r="BA7" s="19"/>
+    </row>
+    <row r="8" spans="1:54" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="29">
         <v>1.5</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="21" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="5">
@@ -1568,103 +1696,118 @@
       <c r="AG8" s="3"/>
       <c r="AL8" s="3"/>
       <c r="AQ8" s="3"/>
-    </row>
-    <row r="9" spans="1:43" s="21" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="33">
+      <c r="BA8" s="3"/>
+    </row>
+    <row r="9" spans="1:54" s="18" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="30">
         <v>1.6</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="17">
         <v>1</v>
       </c>
       <c r="F9" s="13"/>
-      <c r="H9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="R9" s="22"/>
-      <c r="W9" s="22"/>
-      <c r="AB9" s="22"/>
-      <c r="AG9" s="22"/>
-      <c r="AL9" s="22"/>
-      <c r="AQ9" s="22"/>
-    </row>
-    <row r="10" spans="1:43" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="32">
+      <c r="H9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="W9" s="19"/>
+      <c r="AB9" s="19"/>
+      <c r="AG9" s="19"/>
+      <c r="AL9" s="19"/>
+      <c r="AQ9" s="19"/>
+      <c r="AV9" s="19"/>
+      <c r="BA9" s="19"/>
+    </row>
+    <row r="10" spans="1:54" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="29">
         <v>1.7</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="21" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="67"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="69"/>
-      <c r="H10" s="69"/>
-      <c r="I10" s="69"/>
-      <c r="J10" s="69"/>
-      <c r="K10" s="69"/>
-      <c r="L10" s="69"/>
-      <c r="M10" s="69"/>
-      <c r="N10" s="69"/>
-      <c r="O10" s="69"/>
-      <c r="P10" s="69"/>
-      <c r="Q10" s="69"/>
-      <c r="R10" s="69"/>
-      <c r="S10" s="69"/>
-      <c r="T10" s="69"/>
-      <c r="U10" s="69"/>
-      <c r="V10" s="69"/>
-      <c r="W10" s="69"/>
-      <c r="X10" s="69"/>
-      <c r="Y10" s="69"/>
-      <c r="Z10" s="69"/>
-      <c r="AA10" s="69"/>
-      <c r="AB10" s="69"/>
-      <c r="AC10" s="69"/>
-      <c r="AD10" s="69"/>
-      <c r="AE10" s="69"/>
-      <c r="AF10" s="69"/>
-      <c r="AG10" s="69"/>
-      <c r="AH10" s="69"/>
-      <c r="AI10" s="69"/>
-      <c r="AJ10" s="69"/>
-      <c r="AK10" s="69"/>
-      <c r="AL10" s="69"/>
-      <c r="AM10" s="69"/>
-      <c r="AN10" s="69"/>
-      <c r="AO10" s="68"/>
-      <c r="AQ10" s="3"/>
-    </row>
-    <row r="11" spans="1:43" s="21" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="33">
+      <c r="E10" s="42"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="43"/>
+      <c r="S10" s="43"/>
+      <c r="T10" s="43"/>
+      <c r="U10" s="43"/>
+      <c r="V10" s="43"/>
+      <c r="W10" s="43"/>
+      <c r="X10" s="43"/>
+      <c r="Y10" s="43"/>
+      <c r="Z10" s="43"/>
+      <c r="AA10" s="43"/>
+      <c r="AB10" s="43"/>
+      <c r="AC10" s="43"/>
+      <c r="AD10" s="43"/>
+      <c r="AE10" s="43"/>
+      <c r="AF10" s="43"/>
+      <c r="AG10" s="43"/>
+      <c r="AH10" s="43"/>
+      <c r="AI10" s="43"/>
+      <c r="AJ10" s="43"/>
+      <c r="AK10" s="43"/>
+      <c r="AL10" s="43"/>
+      <c r="AM10" s="43"/>
+      <c r="AN10" s="43"/>
+      <c r="AO10" s="43"/>
+      <c r="AP10" s="43"/>
+      <c r="AQ10" s="43"/>
+      <c r="AR10" s="43"/>
+      <c r="AS10" s="43"/>
+      <c r="AT10" s="43"/>
+      <c r="AU10" s="43"/>
+      <c r="AV10" s="43"/>
+      <c r="AW10" s="43"/>
+      <c r="AX10" s="43"/>
+      <c r="AY10" s="44"/>
+      <c r="BA10" s="3"/>
+    </row>
+    <row r="11" spans="1:54" s="18" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="30">
         <v>1.8</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="17">
         <v>4</v>
       </c>
-      <c r="F11" s="67"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="68"/>
-      <c r="M11" s="22"/>
-      <c r="R11" s="22"/>
-      <c r="W11" s="22"/>
-      <c r="AB11" s="22"/>
-      <c r="AG11" s="22"/>
-      <c r="AL11" s="22"/>
-      <c r="AQ11" s="22"/>
-    </row>
-    <row r="12" spans="1:43" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="32">
+      <c r="F11" s="46"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="77"/>
+      <c r="I11" s="47"/>
+      <c r="M11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="W11" s="19"/>
+      <c r="AB11" s="19"/>
+      <c r="AG11" s="19"/>
+      <c r="AL11" s="19"/>
+      <c r="AQ11" s="19"/>
+      <c r="AV11" s="19"/>
+      <c r="BA11" s="19"/>
+    </row>
+    <row r="12" spans="1:54" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="29">
         <v>1.9</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="21" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="5">
@@ -1679,41 +1822,44 @@
       <c r="AG12" s="3"/>
       <c r="AL12" s="3"/>
       <c r="AQ12" s="3"/>
-    </row>
-    <row r="13" spans="1:43" s="21" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="33">
+      <c r="BA12" s="3"/>
+    </row>
+    <row r="13" spans="1:54" s="18" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="30">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="17">
         <v>2</v>
       </c>
-      <c r="F13" s="76"/>
-      <c r="G13" s="77"/>
-      <c r="H13" s="22"/>
-      <c r="M13" s="22"/>
-      <c r="R13" s="22"/>
-      <c r="W13" s="22"/>
-      <c r="AB13" s="22"/>
-      <c r="AG13" s="22"/>
-      <c r="AL13" s="22"/>
-      <c r="AQ13" s="22"/>
-    </row>
-    <row r="14" spans="1:43" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="32">
+      <c r="F13" s="48"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="W13" s="19"/>
+      <c r="AB13" s="19"/>
+      <c r="AG13" s="19"/>
+      <c r="AL13" s="19"/>
+      <c r="AQ13" s="19"/>
+      <c r="AV13" s="19"/>
+      <c r="BA13" s="19"/>
+    </row>
+    <row r="14" spans="1:54" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="29">
         <v>1.1100000000000001</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="21" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="5">
         <v>3</v>
       </c>
-      <c r="F14" s="67"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="68"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="44"/>
       <c r="M14" s="3"/>
       <c r="R14" s="3"/>
       <c r="W14" s="3"/>
@@ -1721,39 +1867,42 @@
       <c r="AG14" s="3"/>
       <c r="AL14" s="3"/>
       <c r="AQ14" s="3"/>
-    </row>
-    <row r="15" spans="1:43" s="21" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="33">
+      <c r="BA14" s="3"/>
+    </row>
+    <row r="15" spans="1:54" s="18" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="30">
         <v>1.1200000000000001</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="17">
         <v>1</v>
       </c>
       <c r="F15" s="13"/>
-      <c r="H15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="R15" s="22"/>
-      <c r="W15" s="22"/>
-      <c r="AB15" s="22"/>
-      <c r="AG15" s="22"/>
-      <c r="AL15" s="22"/>
-      <c r="AQ15" s="22"/>
-    </row>
-    <row r="16" spans="1:43" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="32">
+      <c r="H15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="W15" s="19"/>
+      <c r="AB15" s="19"/>
+      <c r="AG15" s="19"/>
+      <c r="AL15" s="19"/>
+      <c r="AQ15" s="19"/>
+      <c r="AV15" s="19"/>
+      <c r="BA15" s="19"/>
+    </row>
+    <row r="16" spans="1:54" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="29">
         <v>1.1299999999999999</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="5">
         <v>2</v>
       </c>
-      <c r="F16" s="67"/>
-      <c r="G16" s="68"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="44"/>
       <c r="H16" s="3"/>
       <c r="M16" s="3"/>
       <c r="R16" s="3"/>
@@ -1762,101 +1911,116 @@
       <c r="AG16" s="3"/>
       <c r="AL16" s="3"/>
       <c r="AQ16" s="3"/>
-    </row>
-    <row r="17" spans="1:43" s="21" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="33">
+      <c r="BA16" s="3"/>
+    </row>
+    <row r="17" spans="1:53" s="18" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="30">
         <v>1.1399999999999999</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C17" s="17">
         <v>1</v>
       </c>
       <c r="F17" s="13"/>
-      <c r="H17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="R17" s="22"/>
-      <c r="W17" s="22"/>
-      <c r="AB17" s="22"/>
-      <c r="AG17" s="22"/>
-      <c r="AL17" s="22"/>
-      <c r="AQ17" s="22"/>
-    </row>
-    <row r="18" spans="1:43" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="32">
+      <c r="H17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="W17" s="19"/>
+      <c r="AB17" s="19"/>
+      <c r="AG17" s="19"/>
+      <c r="AL17" s="19"/>
+      <c r="AQ17" s="19"/>
+      <c r="AV17" s="19"/>
+      <c r="BA17" s="19"/>
+    </row>
+    <row r="18" spans="1:53" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="29">
         <v>1.1499999999999999</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="21" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="67"/>
-      <c r="G18" s="69"/>
-      <c r="H18" s="69"/>
-      <c r="I18" s="69"/>
-      <c r="J18" s="69"/>
-      <c r="K18" s="69"/>
-      <c r="L18" s="69"/>
-      <c r="M18" s="69"/>
-      <c r="N18" s="69"/>
-      <c r="O18" s="69"/>
-      <c r="P18" s="69"/>
-      <c r="Q18" s="69"/>
-      <c r="R18" s="69"/>
-      <c r="S18" s="69"/>
-      <c r="T18" s="69"/>
-      <c r="U18" s="69"/>
-      <c r="V18" s="69"/>
-      <c r="W18" s="69"/>
-      <c r="X18" s="69"/>
-      <c r="Y18" s="69"/>
-      <c r="Z18" s="69"/>
-      <c r="AA18" s="69"/>
-      <c r="AB18" s="69"/>
-      <c r="AC18" s="69"/>
-      <c r="AD18" s="69"/>
-      <c r="AE18" s="69"/>
-      <c r="AF18" s="69"/>
-      <c r="AG18" s="69"/>
-      <c r="AH18" s="69"/>
-      <c r="AI18" s="69"/>
-      <c r="AJ18" s="69"/>
-      <c r="AK18" s="69"/>
-      <c r="AL18" s="69"/>
-      <c r="AM18" s="69"/>
-      <c r="AN18" s="69"/>
-      <c r="AO18" s="68"/>
-      <c r="AQ18" s="3"/>
-    </row>
-    <row r="19" spans="1:43" s="21" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="33">
+      <c r="F18" s="42"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="43"/>
+      <c r="M18" s="43"/>
+      <c r="N18" s="43"/>
+      <c r="O18" s="43"/>
+      <c r="P18" s="43"/>
+      <c r="Q18" s="43"/>
+      <c r="R18" s="43"/>
+      <c r="S18" s="43"/>
+      <c r="T18" s="43"/>
+      <c r="U18" s="43"/>
+      <c r="V18" s="43"/>
+      <c r="W18" s="43"/>
+      <c r="X18" s="43"/>
+      <c r="Y18" s="43"/>
+      <c r="Z18" s="43"/>
+      <c r="AA18" s="43"/>
+      <c r="AB18" s="43"/>
+      <c r="AC18" s="43"/>
+      <c r="AD18" s="43"/>
+      <c r="AE18" s="43"/>
+      <c r="AF18" s="43"/>
+      <c r="AG18" s="43"/>
+      <c r="AH18" s="43"/>
+      <c r="AI18" s="43"/>
+      <c r="AJ18" s="43"/>
+      <c r="AK18" s="43"/>
+      <c r="AL18" s="43"/>
+      <c r="AM18" s="43"/>
+      <c r="AN18" s="43"/>
+      <c r="AO18" s="43"/>
+      <c r="AP18" s="43"/>
+      <c r="AQ18" s="43"/>
+      <c r="AR18" s="43"/>
+      <c r="AS18" s="43"/>
+      <c r="AT18" s="43"/>
+      <c r="AU18" s="43"/>
+      <c r="AV18" s="43"/>
+      <c r="AW18" s="43"/>
+      <c r="AX18" s="43"/>
+      <c r="AY18" s="44"/>
+      <c r="BA18" s="3"/>
+    </row>
+    <row r="19" spans="1:53" s="18" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="30">
         <v>1.1599999999999999</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C19" s="17">
         <v>2</v>
       </c>
-      <c r="F19" s="67"/>
-      <c r="G19" s="68"/>
-      <c r="H19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="R19" s="22"/>
-      <c r="W19" s="22"/>
-      <c r="AB19" s="22"/>
-      <c r="AG19" s="22"/>
-      <c r="AL19" s="22"/>
-      <c r="AQ19" s="22"/>
-    </row>
-    <row r="20" spans="1:43" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="32">
+      <c r="F19" s="46"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="R19" s="19"/>
+      <c r="W19" s="19"/>
+      <c r="AB19" s="19"/>
+      <c r="AG19" s="19"/>
+      <c r="AL19" s="19"/>
+      <c r="AQ19" s="19"/>
+      <c r="AV19" s="19"/>
+      <c r="BA19" s="19"/>
+    </row>
+    <row r="20" spans="1:53" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="29">
         <v>1.17</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="21" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="5">
@@ -1871,88 +2035,94 @@
       <c r="AG20" s="3"/>
       <c r="AL20" s="3"/>
       <c r="AQ20" s="3"/>
-    </row>
-    <row r="21" spans="1:43" s="21" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="33">
+      <c r="BA20" s="3"/>
+    </row>
+    <row r="21" spans="1:53" s="18" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="30">
         <v>1.18</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="20">
+      <c r="C21" s="17">
         <v>1</v>
       </c>
       <c r="F21" s="12"/>
-      <c r="H21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="R21" s="22"/>
-      <c r="W21" s="22"/>
-      <c r="AB21" s="22"/>
-      <c r="AG21" s="22"/>
-      <c r="AL21" s="22"/>
-      <c r="AQ21" s="22"/>
-    </row>
-    <row r="22" spans="1:43" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="34" t="s">
+      <c r="H21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="R21" s="19"/>
+      <c r="W21" s="19"/>
+      <c r="AB21" s="19"/>
+      <c r="AG21" s="19"/>
+      <c r="AL21" s="19"/>
+      <c r="AQ21" s="19"/>
+      <c r="AV21" s="19"/>
+      <c r="BA21" s="19"/>
+    </row>
+    <row r="22" spans="1:53" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="23" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="7"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="70"/>
-      <c r="J22" s="71"/>
-      <c r="K22" s="71"/>
-      <c r="L22" s="71"/>
-      <c r="M22" s="71"/>
-      <c r="N22" s="71"/>
-      <c r="O22" s="71"/>
-      <c r="P22" s="71"/>
-      <c r="Q22" s="71"/>
-      <c r="R22" s="72"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="54"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="54"/>
+      <c r="M22" s="54"/>
+      <c r="N22" s="54"/>
+      <c r="O22" s="54"/>
+      <c r="P22" s="54"/>
+      <c r="Q22" s="54"/>
+      <c r="R22" s="55"/>
       <c r="W22" s="3"/>
       <c r="AB22" s="3"/>
       <c r="AG22" s="3"/>
       <c r="AL22" s="3"/>
       <c r="AQ22" s="3"/>
-    </row>
-    <row r="23" spans="1:43" s="21" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="33">
+      <c r="BA22" s="3"/>
+    </row>
+    <row r="23" spans="1:53" s="18" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="30">
         <v>2.1</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="20">
+      <c r="C23" s="17">
         <v>4</v>
       </c>
-      <c r="H23" s="22"/>
-      <c r="I23" s="60"/>
-      <c r="J23" s="73"/>
-      <c r="K23" s="73"/>
-      <c r="L23" s="61"/>
-      <c r="M23" s="22"/>
-      <c r="R23" s="22"/>
-      <c r="W23" s="22"/>
-      <c r="AB23" s="22"/>
-      <c r="AG23" s="22"/>
-      <c r="AL23" s="22"/>
-      <c r="AQ23" s="22"/>
-    </row>
-    <row r="24" spans="1:43" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="32">
+      <c r="H23" s="19"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="57"/>
+      <c r="K23" s="57"/>
+      <c r="L23" s="58"/>
+      <c r="M23" s="19"/>
+      <c r="R23" s="19"/>
+      <c r="W23" s="19"/>
+      <c r="AB23" s="19"/>
+      <c r="AG23" s="19"/>
+      <c r="AL23" s="19"/>
+      <c r="AQ23" s="19"/>
+      <c r="AV23" s="19"/>
+      <c r="BA23" s="19"/>
+    </row>
+    <row r="24" spans="1:53" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="29">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="21" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="5">
         <v>2</v>
       </c>
       <c r="H24" s="3"/>
-      <c r="I24" s="60"/>
-      <c r="J24" s="61"/>
+      <c r="I24" s="56"/>
+      <c r="J24" s="58"/>
       <c r="M24" s="3"/>
       <c r="R24" s="3"/>
       <c r="W24" s="3"/>
@@ -1960,33 +2130,36 @@
       <c r="AG24" s="3"/>
       <c r="AL24" s="3"/>
       <c r="AQ24" s="3"/>
-    </row>
-    <row r="25" spans="1:43" s="21" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="33">
+      <c r="BA24" s="3"/>
+    </row>
+    <row r="25" spans="1:53" s="18" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="30">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="20">
+      <c r="C25" s="17">
         <v>3</v>
       </c>
-      <c r="H25" s="22"/>
-      <c r="M25" s="62"/>
-      <c r="N25" s="61"/>
-      <c r="O25" s="61"/>
-      <c r="R25" s="22"/>
-      <c r="W25" s="22"/>
-      <c r="AB25" s="22"/>
-      <c r="AG25" s="22"/>
-      <c r="AL25" s="22"/>
-      <c r="AQ25" s="22"/>
-    </row>
-    <row r="26" spans="1:43" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="32">
+      <c r="H25" s="19"/>
+      <c r="M25" s="59"/>
+      <c r="N25" s="58"/>
+      <c r="O25" s="58"/>
+      <c r="R25" s="19"/>
+      <c r="W25" s="19"/>
+      <c r="AB25" s="19"/>
+      <c r="AG25" s="19"/>
+      <c r="AL25" s="19"/>
+      <c r="AQ25" s="19"/>
+      <c r="AV25" s="19"/>
+      <c r="BA25" s="19"/>
+    </row>
+    <row r="26" spans="1:53" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="29">
         <v>2.4</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="21" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="5">
@@ -1994,41 +2167,44 @@
       </c>
       <c r="H26" s="3"/>
       <c r="M26" s="3"/>
-      <c r="P26" s="60"/>
-      <c r="Q26" s="61"/>
+      <c r="P26" s="56"/>
+      <c r="Q26" s="58"/>
       <c r="R26" s="3"/>
       <c r="W26" s="3"/>
       <c r="AB26" s="3"/>
       <c r="AG26" s="3"/>
       <c r="AL26" s="3"/>
       <c r="AQ26" s="3"/>
-    </row>
-    <row r="27" spans="1:43" s="21" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="33">
+      <c r="BA26" s="3"/>
+    </row>
+    <row r="27" spans="1:53" s="18" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="30">
         <v>2.5</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="20">
+      <c r="C27" s="17">
         <v>2</v>
       </c>
-      <c r="H27" s="22"/>
-      <c r="I27" s="60"/>
-      <c r="J27" s="61"/>
-      <c r="M27" s="22"/>
-      <c r="R27" s="22"/>
-      <c r="W27" s="22"/>
-      <c r="AB27" s="22"/>
-      <c r="AG27" s="22"/>
-      <c r="AL27" s="22"/>
-      <c r="AQ27" s="22"/>
-    </row>
-    <row r="28" spans="1:43" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="32">
+      <c r="H27" s="19"/>
+      <c r="I27" s="56"/>
+      <c r="J27" s="58"/>
+      <c r="M27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="W27" s="19"/>
+      <c r="AB27" s="19"/>
+      <c r="AG27" s="19"/>
+      <c r="AL27" s="19"/>
+      <c r="AQ27" s="19"/>
+      <c r="AV27" s="19"/>
+      <c r="BA27" s="19"/>
+    </row>
+    <row r="28" spans="1:53" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="29">
         <v>2.6</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="21" t="s">
         <v>27</v>
       </c>
       <c r="C28" s="5">
@@ -2042,37 +2218,40 @@
       <c r="AG28" s="3"/>
       <c r="AL28" s="3"/>
       <c r="AQ28" s="3"/>
-    </row>
-    <row r="29" spans="1:43" s="21" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="35" t="s">
+      <c r="BA28" s="3"/>
+    </row>
+    <row r="29" spans="1:53" s="18" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="24" t="s">
         <v>28</v>
       </c>
       <c r="C29" s="8"/>
-      <c r="H29" s="22"/>
-      <c r="M29" s="22"/>
-      <c r="R29" s="22"/>
-      <c r="S29" s="63"/>
-      <c r="T29" s="64"/>
-      <c r="U29" s="64"/>
-      <c r="V29" s="64"/>
-      <c r="W29" s="64"/>
-      <c r="X29" s="64"/>
-      <c r="Y29" s="64"/>
-      <c r="Z29" s="64"/>
-      <c r="AA29" s="64"/>
-      <c r="AB29" s="65"/>
-      <c r="AG29" s="22"/>
-      <c r="AL29" s="22"/>
-      <c r="AQ29" s="22"/>
-    </row>
-    <row r="30" spans="1:43" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="32">
+      <c r="H29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="60"/>
+      <c r="T29" s="61"/>
+      <c r="U29" s="61"/>
+      <c r="V29" s="61"/>
+      <c r="W29" s="61"/>
+      <c r="X29" s="61"/>
+      <c r="Y29" s="61"/>
+      <c r="Z29" s="61"/>
+      <c r="AA29" s="61"/>
+      <c r="AB29" s="62"/>
+      <c r="AG29" s="19"/>
+      <c r="AL29" s="19"/>
+      <c r="AQ29" s="19"/>
+      <c r="AV29" s="19"/>
+      <c r="BA29" s="19"/>
+    </row>
+    <row r="30" spans="1:53" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="29">
         <v>3.1</v>
       </c>
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="21" t="s">
         <v>29</v>
       </c>
       <c r="C30" s="5">
@@ -2083,28 +2262,29 @@
       <c r="R30" s="3"/>
       <c r="S30" s="50"/>
       <c r="T30" s="51"/>
-      <c r="U30" s="52"/>
-      <c r="V30" s="52"/>
-      <c r="W30" s="52"/>
-      <c r="X30" s="53"/>
+      <c r="U30" s="63"/>
+      <c r="V30" s="63"/>
+      <c r="W30" s="63"/>
+      <c r="X30" s="64"/>
       <c r="AB30" s="3"/>
       <c r="AG30" s="3"/>
       <c r="AL30" s="3"/>
       <c r="AQ30" s="3"/>
-    </row>
-    <row r="31" spans="1:43" s="21" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="33">
+      <c r="BA30" s="3"/>
+    </row>
+    <row r="31" spans="1:53" s="18" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="30">
         <v>3.2</v>
       </c>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="20">
+      <c r="C31" s="17">
         <v>8</v>
       </c>
-      <c r="H31" s="22"/>
-      <c r="M31" s="22"/>
-      <c r="R31" s="22"/>
+      <c r="H31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="R31" s="19"/>
       <c r="U31" s="50"/>
       <c r="V31" s="51"/>
       <c r="W31" s="51"/>
@@ -2112,16 +2292,18 @@
       <c r="Y31" s="51"/>
       <c r="Z31" s="51"/>
       <c r="AA31" s="51"/>
-      <c r="AB31" s="66"/>
-      <c r="AG31" s="22"/>
-      <c r="AL31" s="22"/>
-      <c r="AQ31" s="22"/>
-    </row>
-    <row r="32" spans="1:43" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="32">
+      <c r="AB31" s="52"/>
+      <c r="AG31" s="19"/>
+      <c r="AL31" s="19"/>
+      <c r="AQ31" s="19"/>
+      <c r="AV31" s="19"/>
+      <c r="BA31" s="19"/>
+    </row>
+    <row r="32" spans="1:53" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="29">
         <v>3.3</v>
       </c>
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="21" t="s">
         <v>31</v>
       </c>
       <c r="C32" s="5">
@@ -2133,46 +2315,49 @@
       <c r="W32" s="3"/>
       <c r="Y32" s="50"/>
       <c r="Z32" s="51"/>
-      <c r="AA32" s="52"/>
-      <c r="AB32" s="53"/>
+      <c r="AA32" s="63"/>
+      <c r="AB32" s="64"/>
       <c r="AG32" s="3"/>
       <c r="AL32" s="3"/>
       <c r="AQ32" s="3"/>
-    </row>
-    <row r="33" spans="1:43" s="21" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="36" t="s">
+      <c r="BA32" s="3"/>
+    </row>
+    <row r="33" spans="1:53" s="18" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="25" t="s">
         <v>32</v>
       </c>
       <c r="C33" s="9"/>
-      <c r="H33" s="22"/>
-      <c r="M33" s="22"/>
-      <c r="R33" s="22"/>
-      <c r="W33" s="22"/>
-      <c r="AA33" s="54"/>
-      <c r="AB33" s="55"/>
-      <c r="AC33" s="55"/>
-      <c r="AD33" s="55"/>
-      <c r="AE33" s="55"/>
-      <c r="AF33" s="55"/>
-      <c r="AG33" s="55"/>
-      <c r="AH33" s="55"/>
-      <c r="AI33" s="55"/>
-      <c r="AJ33" s="55"/>
-      <c r="AK33" s="55"/>
-      <c r="AL33" s="55"/>
-      <c r="AM33" s="55"/>
-      <c r="AN33" s="55"/>
-      <c r="AO33" s="56"/>
-      <c r="AQ33" s="22"/>
-    </row>
-    <row r="34" spans="1:43" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="32">
+      <c r="H33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="R33" s="19"/>
+      <c r="W33" s="19"/>
+      <c r="AA33" s="69"/>
+      <c r="AB33" s="70"/>
+      <c r="AC33" s="70"/>
+      <c r="AD33" s="70"/>
+      <c r="AE33" s="70"/>
+      <c r="AF33" s="70"/>
+      <c r="AG33" s="70"/>
+      <c r="AH33" s="70"/>
+      <c r="AI33" s="70"/>
+      <c r="AJ33" s="70"/>
+      <c r="AK33" s="70"/>
+      <c r="AL33" s="70"/>
+      <c r="AM33" s="70"/>
+      <c r="AN33" s="70"/>
+      <c r="AO33" s="71"/>
+      <c r="AQ33" s="19"/>
+      <c r="AV33" s="19"/>
+      <c r="BA33" s="19"/>
+    </row>
+    <row r="34" spans="1:53" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="29">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B34" s="24" t="s">
+      <c r="B34" s="21" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="5">
@@ -2182,40 +2367,43 @@
       <c r="M34" s="3"/>
       <c r="R34" s="3"/>
       <c r="W34" s="3"/>
-      <c r="AA34" s="57"/>
-      <c r="AB34" s="58"/>
-      <c r="AC34" s="59"/>
+      <c r="AA34" s="72"/>
+      <c r="AB34" s="73"/>
+      <c r="AC34" s="74"/>
       <c r="AG34" s="3"/>
       <c r="AL34" s="3"/>
       <c r="AQ34" s="3"/>
-    </row>
-    <row r="35" spans="1:43" s="21" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="33">
+      <c r="BA34" s="3"/>
+    </row>
+    <row r="35" spans="1:53" s="18" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="30">
         <v>4.2</v>
       </c>
-      <c r="B35" s="25" t="s">
+      <c r="B35" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="20">
+      <c r="C35" s="17">
         <v>4</v>
       </c>
-      <c r="H35" s="22"/>
-      <c r="M35" s="22"/>
-      <c r="R35" s="22"/>
-      <c r="W35" s="22"/>
-      <c r="AA35" s="45"/>
-      <c r="AB35" s="46"/>
-      <c r="AC35" s="46"/>
-      <c r="AD35" s="59"/>
-      <c r="AG35" s="22"/>
-      <c r="AL35" s="22"/>
-      <c r="AQ35" s="22"/>
-    </row>
-    <row r="36" spans="1:43" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="32">
+      <c r="H35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="R35" s="19"/>
+      <c r="W35" s="19"/>
+      <c r="AA35" s="65"/>
+      <c r="AB35" s="66"/>
+      <c r="AC35" s="66"/>
+      <c r="AD35" s="74"/>
+      <c r="AG35" s="19"/>
+      <c r="AL35" s="19"/>
+      <c r="AQ35" s="19"/>
+      <c r="AV35" s="19"/>
+      <c r="BA35" s="19"/>
+    </row>
+    <row r="36" spans="1:53" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="29">
         <v>4.3</v>
       </c>
-      <c r="B36" s="24" t="s">
+      <c r="B36" s="21" t="s">
         <v>35</v>
       </c>
       <c r="C36" s="5">
@@ -2226,42 +2414,45 @@
       <c r="R36" s="3"/>
       <c r="W36" s="3"/>
       <c r="AB36" s="3"/>
-      <c r="AD36" s="57"/>
-      <c r="AE36" s="58"/>
-      <c r="AF36" s="46"/>
-      <c r="AG36" s="46"/>
-      <c r="AH36" s="46"/>
-      <c r="AI36" s="47"/>
+      <c r="AD36" s="72"/>
+      <c r="AE36" s="73"/>
+      <c r="AF36" s="66"/>
+      <c r="AG36" s="66"/>
+      <c r="AH36" s="66"/>
+      <c r="AI36" s="67"/>
       <c r="AL36" s="3"/>
       <c r="AQ36" s="3"/>
-    </row>
-    <row r="37" spans="1:43" s="21" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="33">
+      <c r="BA36" s="3"/>
+    </row>
+    <row r="37" spans="1:53" s="18" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="30">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B37" s="25" t="s">
+      <c r="B37" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="20">
+      <c r="C37" s="17">
         <v>3</v>
       </c>
-      <c r="H37" s="22"/>
-      <c r="M37" s="22"/>
-      <c r="R37" s="22"/>
-      <c r="W37" s="22"/>
-      <c r="AB37" s="22"/>
-      <c r="AC37" s="45"/>
-      <c r="AD37" s="58"/>
-      <c r="AE37" s="59"/>
-      <c r="AG37" s="22"/>
-      <c r="AL37" s="22"/>
-      <c r="AQ37" s="22"/>
-    </row>
-    <row r="38" spans="1:43" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="32">
+      <c r="H37" s="19"/>
+      <c r="M37" s="19"/>
+      <c r="R37" s="19"/>
+      <c r="W37" s="19"/>
+      <c r="AB37" s="19"/>
+      <c r="AC37" s="65"/>
+      <c r="AD37" s="73"/>
+      <c r="AE37" s="74"/>
+      <c r="AG37" s="19"/>
+      <c r="AL37" s="19"/>
+      <c r="AQ37" s="19"/>
+      <c r="AV37" s="19"/>
+      <c r="BA37" s="19"/>
+    </row>
+    <row r="38" spans="1:53" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="29">
         <v>4.5</v>
       </c>
-      <c r="B38" s="24" t="s">
+      <c r="B38" s="21" t="s">
         <v>36</v>
       </c>
       <c r="C38" s="6" t="s">
@@ -2272,46 +2463,49 @@
       <c r="R38" s="3"/>
       <c r="W38" s="3"/>
       <c r="AB38" s="3"/>
-      <c r="AD38" s="45"/>
-      <c r="AE38" s="46"/>
-      <c r="AF38" s="46"/>
-      <c r="AG38" s="46"/>
-      <c r="AH38" s="46"/>
-      <c r="AI38" s="46"/>
-      <c r="AJ38" s="46"/>
-      <c r="AK38" s="46"/>
-      <c r="AL38" s="46"/>
-      <c r="AM38" s="46"/>
-      <c r="AN38" s="46"/>
-      <c r="AO38" s="47"/>
+      <c r="AD38" s="65"/>
+      <c r="AE38" s="66"/>
+      <c r="AF38" s="66"/>
+      <c r="AG38" s="66"/>
+      <c r="AH38" s="66"/>
+      <c r="AI38" s="66"/>
+      <c r="AJ38" s="66"/>
+      <c r="AK38" s="66"/>
+      <c r="AL38" s="66"/>
+      <c r="AM38" s="66"/>
+      <c r="AN38" s="66"/>
+      <c r="AO38" s="67"/>
       <c r="AQ38" s="3"/>
-    </row>
-    <row r="39" spans="1:43" s="21" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="33">
+      <c r="BA38" s="3"/>
+    </row>
+    <row r="39" spans="1:53" s="18" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="30">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B39" s="25" t="s">
+      <c r="B39" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="20">
+      <c r="C39" s="17">
         <v>2</v>
       </c>
-      <c r="H39" s="22"/>
-      <c r="M39" s="22"/>
-      <c r="R39" s="22"/>
-      <c r="W39" s="22"/>
-      <c r="AB39" s="22"/>
-      <c r="AG39" s="22"/>
-      <c r="AJ39" s="45"/>
-      <c r="AK39" s="47"/>
-      <c r="AL39" s="22"/>
-      <c r="AQ39" s="22"/>
-    </row>
-    <row r="40" spans="1:43" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="37" t="s">
+      <c r="H39" s="19"/>
+      <c r="M39" s="19"/>
+      <c r="R39" s="19"/>
+      <c r="W39" s="19"/>
+      <c r="AB39" s="19"/>
+      <c r="AG39" s="19"/>
+      <c r="AJ39" s="65"/>
+      <c r="AK39" s="67"/>
+      <c r="AL39" s="19"/>
+      <c r="AQ39" s="19"/>
+      <c r="AV39" s="19"/>
+      <c r="BA39" s="19"/>
+    </row>
+    <row r="40" spans="1:53" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="B40" s="29" t="s">
+      <c r="B40" s="26" t="s">
         <v>38</v>
       </c>
       <c r="C40" s="10"/>
@@ -2321,39 +2515,52 @@
       <c r="W40" s="3"/>
       <c r="AB40" s="3"/>
       <c r="AG40" s="3"/>
-      <c r="AL40" s="48"/>
-      <c r="AM40" s="49"/>
-      <c r="AN40" s="49"/>
-      <c r="AQ40" s="3"/>
-    </row>
-    <row r="41" spans="1:43" s="21" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="33">
+      <c r="AL40" s="95"/>
+      <c r="AM40" s="96"/>
+      <c r="AN40" s="96"/>
+      <c r="AO40" s="96"/>
+      <c r="AP40" s="96"/>
+      <c r="AQ40" s="96"/>
+      <c r="AR40" s="96"/>
+      <c r="AS40" s="96"/>
+      <c r="AT40" s="96"/>
+      <c r="AU40" s="68"/>
+      <c r="BA40" s="3"/>
+    </row>
+    <row r="41" spans="1:53" s="18" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="30">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B41" s="25" t="s">
+      <c r="B41" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="H41" s="22"/>
-      <c r="M41" s="22"/>
-      <c r="R41" s="22"/>
-      <c r="W41" s="22"/>
-      <c r="AB41" s="22"/>
-      <c r="AG41" s="22"/>
-      <c r="AL41" s="15"/>
-      <c r="AQ41" s="22"/>
-    </row>
-    <row r="42" spans="1:43" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="32">
+      <c r="C41" s="36">
+        <v>5</v>
+      </c>
+      <c r="H41" s="19"/>
+      <c r="M41" s="19"/>
+      <c r="R41" s="19"/>
+      <c r="W41" s="19"/>
+      <c r="AB41" s="19"/>
+      <c r="AG41" s="19"/>
+      <c r="AL41" s="92"/>
+      <c r="AM41" s="93"/>
+      <c r="AN41" s="93"/>
+      <c r="AO41" s="93"/>
+      <c r="AP41" s="94"/>
+      <c r="AQ41" s="19"/>
+      <c r="AV41" s="19"/>
+      <c r="BA41" s="19"/>
+    </row>
+    <row r="42" spans="1:53" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="29">
         <v>5.2</v>
       </c>
-      <c r="B42" s="24" t="s">
+      <c r="B42" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="6" t="s">
-        <v>62</v>
+      <c r="C42" s="6">
+        <v>2</v>
       </c>
       <c r="H42" s="3"/>
       <c r="M42" s="3"/>
@@ -2361,34 +2568,40 @@
       <c r="W42" s="3"/>
       <c r="AB42" s="3"/>
       <c r="AG42" s="3"/>
-      <c r="AM42" s="15"/>
-      <c r="AQ42" s="3"/>
-    </row>
-    <row r="43" spans="1:43" s="21" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="33">
+      <c r="AL42" s="15"/>
+      <c r="AQ42" s="81"/>
+      <c r="AR42" s="82"/>
+      <c r="BA42" s="3"/>
+    </row>
+    <row r="43" spans="1:53" s="18" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="30">
         <v>5.3</v>
       </c>
-      <c r="B43" s="25" t="s">
+      <c r="B43" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="H43" s="22"/>
-      <c r="M43" s="22"/>
-      <c r="R43" s="22"/>
-      <c r="W43" s="22"/>
-      <c r="AB43" s="22"/>
-      <c r="AG43" s="22"/>
-      <c r="AL43" s="22"/>
-      <c r="AN43" s="15"/>
-      <c r="AQ43" s="22"/>
-    </row>
-    <row r="44" spans="1:43" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="38" t="s">
+      <c r="C43" s="36">
+        <v>3</v>
+      </c>
+      <c r="H43" s="19"/>
+      <c r="M43" s="19"/>
+      <c r="R43" s="19"/>
+      <c r="W43" s="19"/>
+      <c r="AB43" s="19"/>
+      <c r="AG43" s="19"/>
+      <c r="AL43" s="19"/>
+      <c r="AQ43" s="19"/>
+      <c r="AS43" s="83"/>
+      <c r="AT43" s="84"/>
+      <c r="AU43" s="85"/>
+      <c r="AV43" s="19"/>
+      <c r="BA43" s="19"/>
+    </row>
+    <row r="44" spans="1:53" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="B44" s="30" t="s">
+      <c r="B44" s="27" t="s">
         <v>42</v>
       </c>
       <c r="C44" s="11"/>
@@ -2399,83 +2612,157 @@
       <c r="AB44" s="3"/>
       <c r="AG44" s="3"/>
       <c r="AL44" s="3"/>
-      <c r="AO44" s="16"/>
       <c r="AQ44" s="3"/>
-    </row>
-    <row r="45" spans="1:43" s="21" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="42">
+      <c r="AS44" s="86"/>
+      <c r="AT44" s="87"/>
+      <c r="AU44" s="87"/>
+      <c r="AV44" s="87"/>
+      <c r="AW44" s="87"/>
+      <c r="AX44" s="87"/>
+      <c r="AY44" s="88"/>
+      <c r="BA44" s="3"/>
+    </row>
+    <row r="45" spans="1:53" s="18" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="30">
         <v>6.1</v>
       </c>
-      <c r="B45" s="43" t="s">
+      <c r="B45" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="D45" s="40"/>
-      <c r="E45" s="40"/>
-      <c r="F45" s="40"/>
-      <c r="G45" s="40"/>
-      <c r="H45" s="41"/>
-      <c r="I45" s="40"/>
-      <c r="J45" s="40"/>
-      <c r="K45" s="40"/>
-      <c r="L45" s="40"/>
-      <c r="M45" s="41"/>
-      <c r="N45" s="40"/>
-      <c r="O45" s="40"/>
-      <c r="P45" s="40"/>
-      <c r="Q45" s="40"/>
-      <c r="R45" s="41"/>
-      <c r="S45" s="40"/>
-      <c r="T45" s="40"/>
-      <c r="U45" s="40"/>
-      <c r="V45" s="40"/>
-      <c r="W45" s="41"/>
-      <c r="X45" s="40"/>
-      <c r="Y45" s="40"/>
-      <c r="Z45" s="40"/>
-      <c r="AA45" s="40"/>
-      <c r="AB45" s="41"/>
-      <c r="AC45" s="40"/>
-      <c r="AD45" s="40"/>
-      <c r="AE45" s="40"/>
-      <c r="AF45" s="40"/>
-      <c r="AG45" s="41"/>
-      <c r="AH45" s="40"/>
-      <c r="AI45" s="40"/>
-      <c r="AJ45" s="40"/>
-      <c r="AK45" s="40"/>
-      <c r="AL45" s="41"/>
-      <c r="AM45" s="40"/>
-      <c r="AN45" s="40"/>
-      <c r="AO45" s="17"/>
-      <c r="AP45" s="40"/>
-      <c r="AQ45" s="41"/>
+      <c r="C45" s="36">
+        <v>4</v>
+      </c>
+      <c r="D45" s="75"/>
+      <c r="E45" s="75"/>
+      <c r="F45" s="75"/>
+      <c r="G45" s="75"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="75"/>
+      <c r="J45" s="75"/>
+      <c r="K45" s="75"/>
+      <c r="L45" s="75"/>
+      <c r="M45" s="19"/>
+      <c r="N45" s="75"/>
+      <c r="O45" s="75"/>
+      <c r="P45" s="75"/>
+      <c r="Q45" s="75"/>
+      <c r="R45" s="19"/>
+      <c r="S45" s="75"/>
+      <c r="T45" s="75"/>
+      <c r="U45" s="75"/>
+      <c r="V45" s="75"/>
+      <c r="W45" s="19"/>
+      <c r="X45" s="75"/>
+      <c r="Y45" s="75"/>
+      <c r="Z45" s="75"/>
+      <c r="AA45" s="75"/>
+      <c r="AB45" s="19"/>
+      <c r="AC45" s="75"/>
+      <c r="AD45" s="75"/>
+      <c r="AE45" s="75"/>
+      <c r="AF45" s="75"/>
+      <c r="AG45" s="19"/>
+      <c r="AH45" s="75"/>
+      <c r="AI45" s="75"/>
+      <c r="AJ45" s="75"/>
+      <c r="AK45" s="75"/>
+      <c r="AL45" s="19"/>
+      <c r="AM45" s="75"/>
+      <c r="AN45" s="75"/>
+      <c r="AO45" s="75"/>
+      <c r="AP45" s="75"/>
+      <c r="AQ45" s="19"/>
+      <c r="AV45" s="89"/>
+      <c r="AW45" s="90"/>
+      <c r="AX45" s="90"/>
+      <c r="AY45" s="91"/>
+      <c r="BA45" s="19"/>
+    </row>
+    <row r="46" spans="1:53" s="76" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="100" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" s="101" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" s="102">
+        <v>7</v>
+      </c>
+      <c r="D46" s="103"/>
+      <c r="E46" s="98"/>
+      <c r="F46" s="98"/>
+      <c r="G46" s="98"/>
+      <c r="H46" s="98"/>
+      <c r="I46" s="103"/>
+      <c r="J46" s="98"/>
+      <c r="K46" s="98"/>
+      <c r="L46" s="98"/>
+      <c r="M46" s="98"/>
+      <c r="N46" s="103"/>
+      <c r="O46" s="98"/>
+      <c r="P46" s="98"/>
+      <c r="Q46" s="98"/>
+      <c r="R46" s="99"/>
+      <c r="S46" s="98"/>
+      <c r="T46" s="98"/>
+      <c r="U46" s="98"/>
+      <c r="V46" s="98"/>
+      <c r="W46" s="99"/>
+      <c r="X46" s="98"/>
+      <c r="Y46" s="98"/>
+      <c r="Z46" s="98"/>
+      <c r="AA46" s="98"/>
+      <c r="AB46" s="98"/>
+      <c r="AC46" s="103"/>
+      <c r="AD46" s="98"/>
+      <c r="AE46" s="98"/>
+      <c r="AF46" s="98"/>
+      <c r="AG46" s="98"/>
+      <c r="AH46" s="103"/>
+      <c r="AI46" s="98"/>
+      <c r="AJ46" s="98"/>
+      <c r="AK46" s="98"/>
+      <c r="AL46" s="98"/>
+      <c r="AM46" s="103"/>
+      <c r="AN46" s="98"/>
+      <c r="AO46" s="98"/>
+      <c r="AP46" s="98"/>
+      <c r="AQ46" s="98"/>
+      <c r="AR46" s="104"/>
+      <c r="AS46" s="89"/>
+      <c r="AT46" s="90"/>
+      <c r="AU46" s="90"/>
+      <c r="AV46" s="90"/>
+      <c r="AW46" s="90"/>
+      <c r="AX46" s="90"/>
+      <c r="AY46" s="91"/>
+      <c r="AZ46" s="98"/>
+      <c r="BA46" s="99"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="AM1:AQ1"/>
-    <mergeCell ref="D3:AO3"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="I1:M1"/>
-    <mergeCell ref="N1:R1"/>
-    <mergeCell ref="S1:W1"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="X1:AB1"/>
-    <mergeCell ref="AC1:AG1"/>
-    <mergeCell ref="AH1:AL1"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="E10:AO10"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="F13:G13"/>
+  <mergeCells count="47">
+    <mergeCell ref="AW1:BA1"/>
+    <mergeCell ref="D3:AY3"/>
+    <mergeCell ref="E10:AY10"/>
+    <mergeCell ref="AQ42:AR42"/>
+    <mergeCell ref="AS43:AU43"/>
+    <mergeCell ref="AS44:AY44"/>
+    <mergeCell ref="AS46:AY46"/>
+    <mergeCell ref="AV45:AY45"/>
+    <mergeCell ref="AR1:AV1"/>
+    <mergeCell ref="AL41:AP41"/>
+    <mergeCell ref="F18:AY18"/>
+    <mergeCell ref="AL40:AU40"/>
+    <mergeCell ref="AD38:AO38"/>
+    <mergeCell ref="AJ39:AK39"/>
+    <mergeCell ref="Y32:AB32"/>
+    <mergeCell ref="AA33:AO33"/>
+    <mergeCell ref="AA34:AC34"/>
+    <mergeCell ref="AA35:AD35"/>
+    <mergeCell ref="AD36:AI36"/>
+    <mergeCell ref="AC37:AE37"/>
     <mergeCell ref="U31:AB31"/>
     <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F18:AO18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="I22:R22"/>
     <mergeCell ref="I23:L23"/>
@@ -2485,18 +2772,25 @@
     <mergeCell ref="P26:Q26"/>
     <mergeCell ref="S29:AB29"/>
     <mergeCell ref="S30:X30"/>
-    <mergeCell ref="AD38:AO38"/>
-    <mergeCell ref="AJ39:AK39"/>
-    <mergeCell ref="AL40:AN40"/>
-    <mergeCell ref="Y32:AB32"/>
-    <mergeCell ref="AA33:AO33"/>
-    <mergeCell ref="AA34:AC34"/>
-    <mergeCell ref="AA35:AD35"/>
-    <mergeCell ref="AD36:AI36"/>
-    <mergeCell ref="AC37:AE37"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="X1:AB1"/>
+    <mergeCell ref="AC1:AG1"/>
+    <mergeCell ref="AH1:AL1"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="AM1:AQ1"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="I1:M1"/>
+    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="S1:W1"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="45" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="37" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="A44 A40 A33 A29 A22 A3" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>